<commit_message>
Analyse bijgewerkt, klassendiagram toegevoegd, testplan 3/4e uitgewerkt
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -40,19 +40,19 @@
     <t>Use Cases + UCD</t>
   </si>
   <si>
-    <t>ERD + uitloop</t>
-  </si>
-  <si>
-    <t>Testplan</t>
-  </si>
-  <si>
-    <t>strokendiagram</t>
-  </si>
-  <si>
     <t>klassendiagram</t>
   </si>
   <si>
     <t>woensdag 9-12-2015</t>
+  </si>
+  <si>
+    <t>Uitloop</t>
+  </si>
+  <si>
+    <t>ERD</t>
+  </si>
+  <si>
+    <t>testplan + gesprek</t>
   </si>
 </sst>
 </file>
@@ -497,7 +497,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +571,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -582,13 +582,13 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C5" s="9">
-        <v>0.60416666666666663</v>
+        <v>0.59375</v>
       </c>
       <c r="D5" s="3">
         <v>30</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -596,16 +596,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7">
-        <v>0.60416666666666663</v>
+        <v>0.59375</v>
       </c>
       <c r="C6" s="9">
-        <v>0.63541666666666663</v>
+        <v>0.625</v>
       </c>
       <c r="D6" s="3">
         <v>45</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>0.63541666666666663</v>
+        <v>0.625</v>
       </c>
       <c r="C7" s="9">
         <v>0.66666666666666663</v>
@@ -622,12 +622,12 @@
         <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="3"/>
@@ -635,7 +635,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="3"/>
@@ -643,7 +643,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="3"/>

</xml_diff>